<commit_message>
update template user excel
</commit_message>
<xml_diff>
--- a/public/templates/users.xlsx
+++ b/public/templates/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daust\projects\eda\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FCC879-8B70-44E4-9B6C-BD0908746488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D14FDCF-F4BD-40EC-B90A-6F971CB9D2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AE08A987-8248-4635-8A35-4AAEF15862EC}"/>
   </bookViews>
@@ -83,10 +83,10 @@
     <t>Actualizado</t>
   </si>
   <si>
-    <t>Total: 35</t>
-  </si>
-  <si>
     <t>Fecha de Nacimiento</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -102,7 +102,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Aptos Narrow"/>
@@ -112,12 +111,11 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Abadi"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,13 +127,34 @@
         <fgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF012060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -145,23 +164,55 @@
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color theme="1"/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -171,6 +222,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF315496"/>
+      <color rgb="FF012060"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -499,84 +556,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7173D7AD-3810-468A-AE96-F5436B130890}">
-  <dimension ref="B3:Q5"/>
+  <dimension ref="B3:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="5" width="21" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" customWidth="1"/>
-    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="2" max="2" width="8" style="6" customWidth="1"/>
+    <col min="3" max="3" width="4" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15" style="7" customWidth="1"/>
+    <col min="5" max="5" width="21" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21" style="6" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="7"/>
+    <col min="8" max="8" width="12.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="7" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="7"/>
+    <col min="12" max="12" width="14.28515625" style="7" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="7"/>
+    <col min="15" max="15" width="9.140625" style="6"/>
+    <col min="16" max="16" width="9.140625" style="7"/>
+    <col min="17" max="17" width="13.28515625" style="7" customWidth="1"/>
+    <col min="18" max="18" width="12" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2"/>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:18" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:C3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>